<commit_message>
add UDS Forms B5, B6
</commit_message>
<xml_diff>
--- a/WIP__translation_dictionary.xlsx
+++ b/WIP__translation_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ldmay/Box Sync/Documents/MADC_Data_Unification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6209B18-DA56-8E42-A096-4F2A93CF555F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E801A3-3619-5949-8C06-BC9AC88F1505}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="24000" xr2:uid="{35E1C540-DD7A-FA43-A99D-8F94692F3DD6}"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="25600" windowHeight="24000" xr2:uid="{35E1C540-DD7A-FA43-A99D-8F94692F3DD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5436" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5914" uniqueCount="1137">
   <si>
     <t>form_u2</t>
   </si>
@@ -3222,6 +3222,228 @@
   </si>
   <si>
     <t>ivp_b4</t>
+  </si>
+  <si>
+    <t>b5ptid</t>
+  </si>
+  <si>
+    <t>b5pkt_type</t>
+  </si>
+  <si>
+    <t>b5_formver</t>
+  </si>
+  <si>
+    <t>b5_formdate</t>
+  </si>
+  <si>
+    <t>b5_visit_month</t>
+  </si>
+  <si>
+    <t>b5_visit_day</t>
+  </si>
+  <si>
+    <t>b5_visit_yr</t>
+  </si>
+  <si>
+    <t>b5visit_num</t>
+  </si>
+  <si>
+    <t>b5_examiner</t>
+  </si>
+  <si>
+    <t>npiqinf</t>
+  </si>
+  <si>
+    <t>npiqinfx</t>
+  </si>
+  <si>
+    <t>del</t>
+  </si>
+  <si>
+    <t>delsev</t>
+  </si>
+  <si>
+    <t>hall</t>
+  </si>
+  <si>
+    <t>hallsev</t>
+  </si>
+  <si>
+    <t>agit</t>
+  </si>
+  <si>
+    <t>agitsev</t>
+  </si>
+  <si>
+    <t>depd</t>
+  </si>
+  <si>
+    <t>depdsev</t>
+  </si>
+  <si>
+    <t>anx</t>
+  </si>
+  <si>
+    <t>anxsev</t>
+  </si>
+  <si>
+    <t>elat</t>
+  </si>
+  <si>
+    <t>elatsev</t>
+  </si>
+  <si>
+    <t>apa</t>
+  </si>
+  <si>
+    <t>apasev</t>
+  </si>
+  <si>
+    <t>disn</t>
+  </si>
+  <si>
+    <t>disnsev</t>
+  </si>
+  <si>
+    <t>irr</t>
+  </si>
+  <si>
+    <t>irrsev</t>
+  </si>
+  <si>
+    <t>mot</t>
+  </si>
+  <si>
+    <t>motsev</t>
+  </si>
+  <si>
+    <t>nite</t>
+  </si>
+  <si>
+    <t>nitesev</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t>appsev</t>
+  </si>
+  <si>
+    <t>form_b5_behavioral_assessment_npi_q_complete</t>
+  </si>
+  <si>
+    <t>form_b5_behavioral_assessment_npi_q</t>
+  </si>
+  <si>
+    <t>form_b5_behavioral_assessment_npiq_complete</t>
+  </si>
+  <si>
+    <t>form_b5_behavioral_assessment_npiq</t>
+  </si>
+  <si>
+    <t>npiq_score</t>
+  </si>
+  <si>
+    <t>ivp_b5_complete</t>
+  </si>
+  <si>
+    <t>ivp_b5</t>
+  </si>
+  <si>
+    <t>ivp_b6</t>
+  </si>
+  <si>
+    <t>b6ptid</t>
+  </si>
+  <si>
+    <t>b6pkt_type</t>
+  </si>
+  <si>
+    <t>b6_formver</t>
+  </si>
+  <si>
+    <t>b6form_date</t>
+  </si>
+  <si>
+    <t>b6_visit_month</t>
+  </si>
+  <si>
+    <t>b6_visit_day</t>
+  </si>
+  <si>
+    <t>b6_visit_yr</t>
+  </si>
+  <si>
+    <t>b6visit_num</t>
+  </si>
+  <si>
+    <t>b6_examiner</t>
+  </si>
+  <si>
+    <t>nogds___1</t>
+  </si>
+  <si>
+    <t>satis</t>
+  </si>
+  <si>
+    <t>dropact</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>bored</t>
+  </si>
+  <si>
+    <t>spirits</t>
+  </si>
+  <si>
+    <t>afraid</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t>helpless</t>
+  </si>
+  <si>
+    <t>stayhome</t>
+  </si>
+  <si>
+    <t>memprob</t>
+  </si>
+  <si>
+    <t>wondrful</t>
+  </si>
+  <si>
+    <t>wrthless</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>hopeless</t>
+  </si>
+  <si>
+    <t>better</t>
+  </si>
+  <si>
+    <t>gds</t>
+  </si>
+  <si>
+    <t>form_b6_gds_complete</t>
+  </si>
+  <si>
+    <t>form_b6_gds</t>
+  </si>
+  <si>
+    <t>nogds___0</t>
+  </si>
+  <si>
+    <t>nogds</t>
+  </si>
+  <si>
+    <t>ivp_b6_complete</t>
   </si>
 </sst>
 </file>
@@ -3591,19 +3813,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE876574-F5A4-7C48-BC15-5FEB63248101}">
-  <dimension ref="A1:J954"/>
+  <dimension ref="A1:J1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A905" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G944" sqref="G944"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A977" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D995" sqref="D995"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" style="3" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
@@ -21893,6 +22115,1572 @@
         <v>11</v>
       </c>
     </row>
+    <row r="955" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A955" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B955" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C955" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D955" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G955" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I955" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="956" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A956" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B956" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C956" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D956" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G956" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I956" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="957" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A957" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B957" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C957" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D957" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G957" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I957" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="958" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A958" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B958" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C958" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D958" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G958" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I958" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="959" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A959" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B959" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C959" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D959" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G959" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I959" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="960" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A960" s="3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B960" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C960" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D960" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G960" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I960" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="961" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A961" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B961" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C961" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D961" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G961" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I961" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="962" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A962" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B962" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C962" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D962" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G962" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I962" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="963" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A963" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B963" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C963" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D963" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G963" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I963" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="964" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A964" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B964" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C964" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D964" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E964" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F964" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G964" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I964" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="965" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A965" s="3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B965" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C965" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D965" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E965" s="3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F965" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G965" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I965" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="966" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A966" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B966" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C966" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D966" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E966" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F966" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G966" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I966" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="967" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A967" s="3" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B967" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C967" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D967" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E967" s="3" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F967" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G967" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I967" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="968" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A968" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B968" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C968" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D968" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E968" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F968" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G968" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I968" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="969" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A969" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B969" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C969" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D969" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E969" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F969" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G969" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I969" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="970" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A970" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B970" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C970" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D970" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E970" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F970" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G970" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I970" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="971" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A971" s="3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B971" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C971" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D971" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E971" s="3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F971" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G971" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I971" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="972" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A972" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B972" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C972" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D972" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E972" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F972" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G972" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I972" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="973" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A973" s="3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B973" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C973" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D973" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E973" s="3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F973" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G973" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I973" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="974" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A974" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B974" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C974" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D974" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E974" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F974" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G974" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I974" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="975" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A975" s="3" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B975" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C975" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D975" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E975" s="3" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F975" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G975" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I975" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="976" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A976" s="3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B976" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C976" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D976" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E976" s="3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F976" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G976" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I976" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="977" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A977" s="3" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B977" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C977" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D977" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E977" s="3" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F977" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G977" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I977" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="978" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A978" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B978" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C978" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D978" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E978" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F978" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G978" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I978" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="979" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A979" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B979" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C979" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D979" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E979" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F979" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G979" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I979" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="980" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A980" s="3" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B980" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C980" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D980" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E980" s="3" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F980" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G980" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I980" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="981" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A981" s="3" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B981" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C981" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D981" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E981" s="3" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F981" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G981" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I981" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="982" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A982" s="3" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B982" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C982" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D982" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E982" s="3" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F982" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G982" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I982" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="983" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A983" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B983" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C983" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D983" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E983" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F983" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G983" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I983" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="984" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A984" s="3" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B984" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C984" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D984" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E984" s="3" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F984" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G984" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I984" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="985" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A985" s="3" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B985" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C985" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D985" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E985" s="3" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F985" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G985" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I985" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="986" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A986" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B986" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C986" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D986" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E986" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F986" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G986" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I986" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="987" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A987" s="3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B987" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C987" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D987" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E987" s="3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="F987" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G987" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I987" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="988" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A988" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B988" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C988" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D988" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E988" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F988" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G988" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I988" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="989" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A989" s="3" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B989" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C989" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D989" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E989" s="3" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F989" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G989" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I989" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="990" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A990" s="3" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B990" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C990" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D990" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E990" s="3" t="s">
+        <v>1103</v>
+      </c>
+      <c r="F990" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G990" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I990" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="991" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E991" s="3" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F991" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G991" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I991" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="992" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A992" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B992" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C992" s="3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D992" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G992" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I992" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="993" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A993" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B993" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C993" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D993" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G993" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I993" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="994" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A994" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B994" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C994" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D994" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G994" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I994" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="995" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A995" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B995" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C995" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D995" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G995" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I995" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="996" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A996" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B996" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C996" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D996" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G996" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I996" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="997" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A997" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B997" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C997" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D997" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G997" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I997" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="998" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A998" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B998" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C998" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D998" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G998" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I998" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="999" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A999" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B999" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C999" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D999" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G999" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I999" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1000" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1000" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D1000" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G1000" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1000" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1001" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1001" s="3" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D1001" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G1001" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1001" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1002" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1002" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D1002" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1002" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F1002" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1002" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1002" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1003" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1003" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D1003" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1003" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F1003" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1003" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1003" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1004" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1004" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D1004" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1004" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F1004" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1004" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1004" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1005" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1005" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D1005" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1005" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F1005" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1005" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1005" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1006" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1006" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1006" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1006" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F1006" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1006" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1006" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1007" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1007" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D1007" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1007" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F1007" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1007" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1007" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1008" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1008" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D1008" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1008" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F1008" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1008" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1008" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1009" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1009" s="3" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D1009" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1009" s="3" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F1009" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1009" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1009" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1010" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1010" s="3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D1010" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1010" s="3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F1010" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1010" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1010" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1011" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1011" s="3" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D1011" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1011" s="3" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F1011" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1011" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1011" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1012" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1012" s="3" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D1012" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1012" s="3" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F1012" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1012" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1012" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1013" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1013" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D1013" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1013" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F1013" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1013" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1013" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1014" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1014" s="3" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D1014" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1014" s="3" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F1014" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1014" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1014" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1015" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1015" s="3" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D1015" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1015" s="3" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F1015" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1015" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1015" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1016" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1016" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1016" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1016" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F1016" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1016" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1016" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1017" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1017" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D1017" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1017" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F1017" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1017" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1017" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1018" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C1018" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D1018" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1018" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1018" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1018" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1018" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C1019" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D1019" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G1019" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1019" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E1020" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F1020" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G1020" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1020" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add UDS Forms B7, B8
</commit_message>
<xml_diff>
--- a/WIP__translation_dictionary.xlsx
+++ b/WIP__translation_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ldmay/Box Sync/Documents/MADC_Data_Unification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E801A3-3619-5949-8C06-BC9AC88F1505}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CA6AAF-121F-754B-9626-CD28912C978D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="0" windowWidth="25600" windowHeight="24000" xr2:uid="{35E1C540-DD7A-FA43-A99D-8F94692F3DD6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5914" uniqueCount="1137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="1222">
   <si>
     <t>form_u2</t>
   </si>
@@ -3444,6 +3444,261 @@
   </si>
   <si>
     <t>ivp_b6_complete</t>
+  </si>
+  <si>
+    <t>b7ptid</t>
+  </si>
+  <si>
+    <t>b7pkt_type</t>
+  </si>
+  <si>
+    <t>b7_formver</t>
+  </si>
+  <si>
+    <t>b7form_date</t>
+  </si>
+  <si>
+    <t>b7_visit_month</t>
+  </si>
+  <si>
+    <t>b7_visit_day</t>
+  </si>
+  <si>
+    <t>b7_visit_yr</t>
+  </si>
+  <si>
+    <t>b7visit_num</t>
+  </si>
+  <si>
+    <t>b7_examiner</t>
+  </si>
+  <si>
+    <t>bills</t>
+  </si>
+  <si>
+    <t>taxes</t>
+  </si>
+  <si>
+    <t>shopping</t>
+  </si>
+  <si>
+    <t>games</t>
+  </si>
+  <si>
+    <t>stove</t>
+  </si>
+  <si>
+    <t>mealprep</t>
+  </si>
+  <si>
+    <t>events</t>
+  </si>
+  <si>
+    <t>payattn</t>
+  </si>
+  <si>
+    <t>remdates</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>form_b7_functional_assessment_faq_complete</t>
+  </si>
+  <si>
+    <t>form_b7_functional_assessment_faq</t>
+  </si>
+  <si>
+    <t>fas_score</t>
+  </si>
+  <si>
+    <t>ivp_b7_complete</t>
+  </si>
+  <si>
+    <t>ivp_b7</t>
+  </si>
+  <si>
+    <t>b8ptid</t>
+  </si>
+  <si>
+    <t>b8pkt_type</t>
+  </si>
+  <si>
+    <t>b8_formver</t>
+  </si>
+  <si>
+    <t>b8form_date</t>
+  </si>
+  <si>
+    <t>b8_visit_month</t>
+  </si>
+  <si>
+    <t>b8_visit_day</t>
+  </si>
+  <si>
+    <t>b8_visit_yr</t>
+  </si>
+  <si>
+    <t>b8visit_num</t>
+  </si>
+  <si>
+    <t>b8_examiner</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>focldef</t>
+  </si>
+  <si>
+    <t>gaitdis</t>
+  </si>
+  <si>
+    <t>eyemove</t>
+  </si>
+  <si>
+    <t>form_b8_physical_neurological_exam_findings_complete</t>
+  </si>
+  <si>
+    <t>form_b8_physical_neurological_exam_findings</t>
+  </si>
+  <si>
+    <t>normexam</t>
+  </si>
+  <si>
+    <t>parksign</t>
+  </si>
+  <si>
+    <t>resttrl</t>
+  </si>
+  <si>
+    <t>resttrr</t>
+  </si>
+  <si>
+    <t>slowingl</t>
+  </si>
+  <si>
+    <t>slowingr</t>
+  </si>
+  <si>
+    <t>rigidl</t>
+  </si>
+  <si>
+    <t>rigidr</t>
+  </si>
+  <si>
+    <t>brady</t>
+  </si>
+  <si>
+    <t>parkgait</t>
+  </si>
+  <si>
+    <t>postinst</t>
+  </si>
+  <si>
+    <t>cvdsigns</t>
+  </si>
+  <si>
+    <t>cortdef</t>
+  </si>
+  <si>
+    <t>sivdfind</t>
+  </si>
+  <si>
+    <t>cvdmotl</t>
+  </si>
+  <si>
+    <t>cvdmotr</t>
+  </si>
+  <si>
+    <t>cortvisl</t>
+  </si>
+  <si>
+    <t>cortvisr</t>
+  </si>
+  <si>
+    <t>somatl</t>
+  </si>
+  <si>
+    <t>somatr</t>
+  </si>
+  <si>
+    <t>postcort</t>
+  </si>
+  <si>
+    <t>pspcbs</t>
+  </si>
+  <si>
+    <t>eyepsp</t>
+  </si>
+  <si>
+    <t>dyspsp</t>
+  </si>
+  <si>
+    <t>axialpsp</t>
+  </si>
+  <si>
+    <t>gaitpsp</t>
+  </si>
+  <si>
+    <t>apraxsp</t>
+  </si>
+  <si>
+    <t>apraxl</t>
+  </si>
+  <si>
+    <t>apraxr</t>
+  </si>
+  <si>
+    <t>cortsenl</t>
+  </si>
+  <si>
+    <t>cortsenr</t>
+  </si>
+  <si>
+    <t>ataxl</t>
+  </si>
+  <si>
+    <t>ataxr</t>
+  </si>
+  <si>
+    <t>akuebknk</t>
+  </si>
+  <si>
+    <t>alienlmr</t>
+  </si>
+  <si>
+    <t>dystonl</t>
+  </si>
+  <si>
+    <t>dystonr</t>
+  </si>
+  <si>
+    <t>myocllt</t>
+  </si>
+  <si>
+    <t>myoclrt</t>
+  </si>
+  <si>
+    <t>alsfind</t>
+  </si>
+  <si>
+    <t>gaitnph</t>
+  </si>
+  <si>
+    <t>othneur</t>
+  </si>
+  <si>
+    <t>othneurx</t>
+  </si>
+  <si>
+    <t>alienlml</t>
+  </si>
+  <si>
+    <t>ivp_b8_complete</t>
+  </si>
+  <si>
+    <t>ivp_b8</t>
   </si>
 </sst>
 </file>
@@ -3813,19 +4068,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE876574-F5A4-7C48-BC15-5FEB63248101}">
-  <dimension ref="A1:J1020"/>
+  <dimension ref="A1:J1098"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A977" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D995" sqref="D995"/>
+      <pane ySplit="1" topLeftCell="A1060" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1099" sqref="A1099"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
@@ -23681,6 +23936,1608 @@
         <v>11</v>
       </c>
     </row>
+    <row r="1021" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1021" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B1021" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1021" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D1021" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1021" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1021" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1022" s="3" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B1022" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1022" s="3" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D1022" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1022" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1022" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1023" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B1023" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1023" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D1023" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1023" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1023" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1024" s="3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B1024" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1024" s="3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D1024" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1024" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1024" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1025" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B1025" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1025" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1025" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1025" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1025" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1026" s="3" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B1026" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1026" s="3" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D1026" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1026" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1026" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1027" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B1027" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1027" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D1027" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1027" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1027" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1028" s="3" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B1028" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1028" s="3" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D1028" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1028" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1028" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1029" s="3" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B1029" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1029" s="3" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D1029" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1029" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1029" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1030" s="3" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B1030" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1030" s="3" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D1030" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1030" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F1030" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1030" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1030" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1031" s="3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B1031" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1031" s="3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D1031" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1031" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F1031" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1031" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1031" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1032" s="3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B1032" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1032" s="3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D1032" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1032" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F1032" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1032" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1032" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1033" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B1033" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1033" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D1033" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1033" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F1033" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1033" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1033" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1034" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B1034" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1034" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D1034" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1034" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F1034" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1034" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1034" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1035" s="3" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B1035" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1035" s="3" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D1035" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1035" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F1035" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1035" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1035" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1036" s="3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B1036" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1036" s="3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D1036" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1036" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F1036" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1036" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1036" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1037" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B1037" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1037" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D1037" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1037" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F1037" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1037" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1037" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1038" s="3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B1038" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1038" s="3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D1038" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1038" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F1038" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1038" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1038" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1039" s="3" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B1039" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1039" s="3" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D1039" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1039" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F1039" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1039" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1039" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1040" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B1040" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1040" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D1040" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1040" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F1040" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1040" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1040" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E1041" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F1041" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1041" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1041" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1042" s="3" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B1042" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1042" s="3" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D1042" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1042" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1042" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1043" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B1043" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1043" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D1043" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1043" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1043" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1044" s="3" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B1044" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1044" s="3" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D1044" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1044" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1044" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1045" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B1045" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1045" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D1045" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1045" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1045" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1046" s="3" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B1046" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1046" s="3" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D1046" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1046" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1046" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1047" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B1047" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1047" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D1047" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1047" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1047" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1048" s="3" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B1048" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1048" s="3" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D1048" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1048" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1048" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1049" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B1049" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1049" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D1049" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1049" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1049" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1050" s="3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B1050" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1050" s="3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D1050" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1050" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1050" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1051" s="3" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B1051" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1051" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1051" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1052" s="3" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B1052" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1052" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1052" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1053" s="3" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B1053" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1053" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1053" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1054" s="3" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B1054" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1054" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1054" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1055" s="3" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B1055" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C1055" s="3" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D1055" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1055" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F1055" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1055" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1055" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C1056" s="3" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1056" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1056" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F1056" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1056" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1056" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1057" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1057" s="3" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D1057" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1057" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F1057" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1057" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1057" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1058" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1058" s="3" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D1058" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1058" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F1058" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1058" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1058" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1059" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1059" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D1059" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1059" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F1059" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1059" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1059" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1060" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1060" s="3" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D1060" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1060" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F1060" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1060" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1060" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1061" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1061" s="3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D1061" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1061" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F1061" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1061" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1061" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1062" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1062" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D1062" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1062" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F1062" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1062" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1062" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1063" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1063" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D1063" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1063" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F1063" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1063" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1063" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1064" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1064" s="3" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D1064" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1064" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F1064" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1064" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1064" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1065" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1065" s="3" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D1065" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1065" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F1065" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1065" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1065" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1066" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1066" s="3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D1066" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1066" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F1066" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1066" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1066" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1067" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1067" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D1067" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1067" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F1067" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1067" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1067" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1068" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1068" s="3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D1068" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1068" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F1068" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1068" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1068" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1069" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1069" s="3" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D1069" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1069" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F1069" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1069" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1069" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1070" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1070" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D1070" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1070" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F1070" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1070" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1070" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1071" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1071" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D1071" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1071" t="s">
+        <v>1191</v>
+      </c>
+      <c r="F1071" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1071" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1071" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1072" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1072" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D1072" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1072" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F1072" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1072" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1072" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1073" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1073" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D1073" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1073" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F1073" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1073" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1073" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1074" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1074" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D1074" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1074" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F1074" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1074" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1074" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1075" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1075" s="3" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D1075" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1075" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F1075" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1075" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1075" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1076" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1076" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D1076" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1076" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F1076" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1076" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1076" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1077" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1077" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D1077" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1077" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F1077" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1077" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1077" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1078" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1078" s="3" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D1078" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1078" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F1078" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1078" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1078" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1079" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1079" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D1079" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1079" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F1079" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1079" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1079" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1080" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1080" s="3" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D1080" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1080" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F1080" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1080" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1080" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1081" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1081" s="3" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D1081" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1081" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F1081" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1081" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1081" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1082" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1082" s="3" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D1082" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1082" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F1082" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1082" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1082" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1083" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1083" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D1083" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1083" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F1083" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1083" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1083" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1084" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1084" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D1084" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1084" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F1084" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1084" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1084" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1085" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1085" s="3" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D1085" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1085" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F1085" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1085" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1085" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1086" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1086" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D1086" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1086" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F1086" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1086" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1086" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1087" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1087" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D1087" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1087" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F1087" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1087" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1087" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1088" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1088" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D1088" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1088" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F1088" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1088" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1088" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1089" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1089" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D1089" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1089" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F1089" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1089" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1089" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1090" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1090" s="3" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D1090" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1090" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F1090" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1090" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1090" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1091" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1091" s="3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D1091" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1091" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F1091" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1091" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1091" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1092" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1092" s="3" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D1092" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1092" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F1092" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1092" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1092" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1093" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1093" s="3" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D1093" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1093" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F1093" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1093" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1093" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1094" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1094" s="3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D1094" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1094" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F1094" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1094" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1094" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1095" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1095" s="3" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D1095" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1095" t="s">
+        <v>1215</v>
+      </c>
+      <c r="F1095" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1095" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1095" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1096" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1096" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D1096" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1096" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F1096" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1096" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1096" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1097" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1097" s="3" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D1097" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1097" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F1097" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1097" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1097" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1098" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1098" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D1098" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1098" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F1098" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1098" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1098" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add UDS Form B9
</commit_message>
<xml_diff>
--- a/WIP__translation_dictionary.xlsx
+++ b/WIP__translation_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ldmay/Box Sync/Documents/MADC_Data_Unification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CA6AAF-121F-754B-9626-CD28912C978D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921AFE63-6974-A946-AC87-F1B83730AC0C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="25600" windowHeight="24000" xr2:uid="{35E1C540-DD7A-FA43-A99D-8F94692F3DD6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{35E1C540-DD7A-FA43-A99D-8F94692F3DD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="1222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6890" uniqueCount="1299">
   <si>
     <t>form_u2</t>
   </si>
@@ -3699,6 +3699,237 @@
   </si>
   <si>
     <t>ivp_b8</t>
+  </si>
+  <si>
+    <t>b9ptid</t>
+  </si>
+  <si>
+    <t>b9pkt_type</t>
+  </si>
+  <si>
+    <t>b9_formver</t>
+  </si>
+  <si>
+    <t>b9form_date</t>
+  </si>
+  <si>
+    <t>b9_visit_month</t>
+  </si>
+  <si>
+    <t>b9_visit_day</t>
+  </si>
+  <si>
+    <t>b9_visit_yr</t>
+  </si>
+  <si>
+    <t>b9visit_num</t>
+  </si>
+  <si>
+    <t>b9_examiner</t>
+  </si>
+  <si>
+    <t>b9chg</t>
+  </si>
+  <si>
+    <t>decsub</t>
+  </si>
+  <si>
+    <t>decin</t>
+  </si>
+  <si>
+    <t>decclin</t>
+  </si>
+  <si>
+    <t>decage</t>
+  </si>
+  <si>
+    <t>cogmem</t>
+  </si>
+  <si>
+    <t>cogjudg</t>
+  </si>
+  <si>
+    <t>coglang</t>
+  </si>
+  <si>
+    <t>cogvis</t>
+  </si>
+  <si>
+    <t>cogattn</t>
+  </si>
+  <si>
+    <t>cogfluc</t>
+  </si>
+  <si>
+    <t>cogothr</t>
+  </si>
+  <si>
+    <t>cogothrx</t>
+  </si>
+  <si>
+    <t>cogfrst</t>
+  </si>
+  <si>
+    <t>cogfrstx</t>
+  </si>
+  <si>
+    <t>cogmode</t>
+  </si>
+  <si>
+    <t>cogmodex</t>
+  </si>
+  <si>
+    <t>beapathy</t>
+  </si>
+  <si>
+    <t>bedep</t>
+  </si>
+  <si>
+    <t>bevhall</t>
+  </si>
+  <si>
+    <t>bevwell</t>
+  </si>
+  <si>
+    <t>beahall</t>
+  </si>
+  <si>
+    <t>bedel</t>
+  </si>
+  <si>
+    <t>bedisin</t>
+  </si>
+  <si>
+    <t>beirrit</t>
+  </si>
+  <si>
+    <t>beagit</t>
+  </si>
+  <si>
+    <t>beperch</t>
+  </si>
+  <si>
+    <t>berem</t>
+  </si>
+  <si>
+    <t>beothr</t>
+  </si>
+  <si>
+    <t>beothrx</t>
+  </si>
+  <si>
+    <t>befrst</t>
+  </si>
+  <si>
+    <t>befrstx</t>
+  </si>
+  <si>
+    <t>bemode</t>
+  </si>
+  <si>
+    <t>bemodex</t>
+  </si>
+  <si>
+    <t>mogait</t>
+  </si>
+  <si>
+    <t>mofalls</t>
+  </si>
+  <si>
+    <t>motrem</t>
+  </si>
+  <si>
+    <t>moslow</t>
+  </si>
+  <si>
+    <t>mofrst</t>
+  </si>
+  <si>
+    <t>momode</t>
+  </si>
+  <si>
+    <t>momodex</t>
+  </si>
+  <si>
+    <t>momopark</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>frstchg</t>
+  </si>
+  <si>
+    <t>form_b9_clinician_judgment_of_symptoms_complete</t>
+  </si>
+  <si>
+    <t>form_b9_clinician_judgment_of_symptoms</t>
+  </si>
+  <si>
+    <t>decclcog</t>
+  </si>
+  <si>
+    <t>cogori</t>
+  </si>
+  <si>
+    <t>cogfpred</t>
+  </si>
+  <si>
+    <t>cogfprex</t>
+  </si>
+  <si>
+    <t>decclbe</t>
+  </si>
+  <si>
+    <t>bevhago</t>
+  </si>
+  <si>
+    <t>beremago</t>
+  </si>
+  <si>
+    <t>beanx</t>
+  </si>
+  <si>
+    <t>befpred</t>
+  </si>
+  <si>
+    <t>befpredx</t>
+  </si>
+  <si>
+    <t>beage</t>
+  </si>
+  <si>
+    <t>decclmot</t>
+  </si>
+  <si>
+    <t>parkage</t>
+  </si>
+  <si>
+    <t>momoals</t>
+  </si>
+  <si>
+    <t>alsage</t>
+  </si>
+  <si>
+    <t>moage</t>
+  </si>
+  <si>
+    <t>lbdeval</t>
+  </si>
+  <si>
+    <t>ftldeval</t>
+  </si>
+  <si>
+    <t>cogflago</t>
+  </si>
+  <si>
+    <t>b9changes</t>
+  </si>
+  <si>
+    <t>ivp_b9_complete</t>
+  </si>
+  <si>
+    <t>ivp_b9</t>
   </si>
 </sst>
 </file>
@@ -4068,22 +4299,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE876574-F5A4-7C48-BC15-5FEB63248101}">
-  <dimension ref="A1:J1098"/>
+  <dimension ref="A1:J1166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1060" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1099" sqref="A1099"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1098" sqref="I1098:I1166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="76.5" style="3" bestFit="1" customWidth="1"/>
@@ -25338,7 +25569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1089" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1089" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1089" s="3" t="s">
         <v>1209</v>
       </c>
@@ -25358,7 +25589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1090" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1090" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1090" s="3" t="s">
         <v>1210</v>
       </c>
@@ -25378,7 +25609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1091" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1091" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1091" s="3" t="s">
         <v>1211</v>
       </c>
@@ -25398,7 +25629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1092" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1092" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1092" s="3" t="s">
         <v>1212</v>
       </c>
@@ -25418,7 +25649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1093" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1093" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1093" s="3" t="s">
         <v>1213</v>
       </c>
@@ -25438,7 +25669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1094" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1094" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1094" s="3" t="s">
         <v>1214</v>
       </c>
@@ -25458,7 +25689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1095" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1095" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1095" s="3" t="s">
         <v>1215</v>
       </c>
@@ -25478,7 +25709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1096" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1096" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1096" s="3" t="s">
         <v>1216</v>
       </c>
@@ -25498,7 +25729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1097" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1097" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1097" s="3" t="s">
         <v>1217</v>
       </c>
@@ -25518,7 +25749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1098" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1098" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1098" s="3" t="s">
         <v>1218</v>
       </c>
@@ -25535,6 +25766,1624 @@
         <v>9</v>
       </c>
       <c r="I1098" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1099" s="3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B1099" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1099" s="3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D1099" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1099" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1099" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1100" s="3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B1100" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1100" s="3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D1100" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1100" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1101" s="3" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B1101" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1101" s="3" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D1101" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1101" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1101" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1102" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B1102" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1102" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D1102" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1102" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1102" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1103" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B1103" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1103" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D1103" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1103" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1103" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1104" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B1104" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1104" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D1104" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1104" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1104" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1105" s="3" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B1105" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1105" s="3" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D1105" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1105" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1105" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1106" s="3" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B1106" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1106" s="3" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D1106" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1106" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1106" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1107" s="3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B1107" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1107" s="3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D1107" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1107" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1107" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1108" s="3" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B1108" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1108" s="3" t="s">
+        <v>1296</v>
+      </c>
+      <c r="F1108" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1108" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1108" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1109" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B1109" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1109" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D1109" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1109" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F1109" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1109" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1109" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1110" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B1110" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1110" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D1110" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1110" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F1110" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1110" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1111" s="3" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B1111" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1111" s="3" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D1111" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1111" s="3" t="s">
+        <v>1277</v>
+      </c>
+      <c r="F1111" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1111" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1111" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1112" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B1112" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1112" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D1112" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1112" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F1112" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1112" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1112" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1113" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B1113" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1113" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D1113" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1113" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="F1113" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1113" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1113" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1114" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B1114" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1114" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D1114" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1114" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F1114" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1114" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1114" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1115" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B1115" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1115" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D1115" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1115" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F1115" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1115" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1115" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1116" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B1116" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1116" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D1116" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1116" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F1116" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1116" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1116" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1117" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B1117" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1117" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D1117" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1117" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="F1117" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1117" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1117" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1118" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B1118" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1118" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D1118" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1118" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F1118" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1118" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1118" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1119" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B1119" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1119" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D1119" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1119" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="F1119" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1119" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1119" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1120" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B1120" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1120" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D1120" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1120" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="F1120" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1120" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1120" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1121" s="3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B1121" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1121" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D1121" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1121" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="F1121" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1121" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1121" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1122" s="3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B1122" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1122" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D1122" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1122" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F1122" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1122" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1122" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1123" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B1123" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1123" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D1123" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1123" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F1123" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1123" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1123" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1124" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B1124" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1124" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D1124" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1124" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F1124" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1124" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1124" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1125" s="3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B1125" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1125" s="3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D1125" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1125" s="3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F1125" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1125" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1125" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1126" s="3" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B1126" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1126" s="3" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D1126" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1126" s="3" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F1126" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1126" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1126" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1127" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1127" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1127" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D1127" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1127" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="F1127" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1127" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1127" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1128" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B1128" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1128" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D1128" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1128" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F1128" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1128" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1128" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1129" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B1129" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1129" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D1129" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1129" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="F1129" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1129" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1129" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1130" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B1130" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1130" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D1130" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1130" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="F1130" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1130" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1130" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1131" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B1131" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1131" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D1131" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1131" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F1131" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1131" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1131" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1132" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B1132" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1132" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D1132" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1132" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="F1132" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1132" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1132" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1133" s="3" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B1133" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1133" s="3" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D1133" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1133" s="3" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F1133" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1133" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1133" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1134" s="3" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B1134" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1134" s="3" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D1134" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1134" s="3" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F1134" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1134" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1134" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1135" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B1135" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1135" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D1135" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1135" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="F1135" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1135" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1135" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1136" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B1136" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1136" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D1136" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1136" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F1136" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1136" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1136" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1137" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1137" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1137" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D1137" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1137" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="F1137" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1137" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1137" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1138" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B1138" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1138" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D1138" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1138" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F1138" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1138" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1138" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1139" s="3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B1139" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1139" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D1139" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1139" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F1139" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1139" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1139" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1140" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B1140" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1140" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D1140" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1140" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="F1140" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1140" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1140" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1141" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B1141" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1141" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D1141" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1141" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F1141" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1141" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1141" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1142" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1142" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1142" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D1142" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1142" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="F1142" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1142" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1142" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1143" s="3" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B1143" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1143" s="3" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D1143" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1143" s="3" t="s">
+        <v>1266</v>
+      </c>
+      <c r="F1143" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1143" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1143" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1144" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B1144" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1144" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D1144" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1144" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F1144" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1144" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1144" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1145" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B1145" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1145" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D1145" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1145" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="F1145" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1145" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1145" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1146" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1146" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1146" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D1146" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1146" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F1146" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1146" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1146" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1147" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B1147" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1147" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D1147" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1147" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="F1147" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1147" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1147" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1148" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B1148" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1148" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1148" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1148" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F1148" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1148" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1148" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1149" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B1149" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1149" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D1149" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1149" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="F1149" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1149" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1149" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1150" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B1150" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1150" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D1150" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1150" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="F1150" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1150" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1150" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1151" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B1151" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1151" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D1151" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1151" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F1151" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1151" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1151" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1152" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B1152" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1152" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D1152" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1152" s="3" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F1152" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1152" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1152" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1153" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1153" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D1153" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1153" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F1153" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1153" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1153" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1154" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1154" s="3" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D1154" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1154" s="3" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F1154" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1154" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1154" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1155" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1155" s="3" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D1155" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1155" s="3" t="s">
+        <v>1282</v>
+      </c>
+      <c r="F1155" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1155" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1155" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1156" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1156" s="3" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D1156" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1156" s="3" t="s">
+        <v>1283</v>
+      </c>
+      <c r="F1156" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1156" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1156" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1157" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1157" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D1157" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1157" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F1157" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1157" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1157" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1158" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1158" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D1158" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1158" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="F1158" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1158" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1158" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1159" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1159" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D1159" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1159" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F1159" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1159" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1159" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1160" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1160" s="3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D1160" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1160" s="3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F1160" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1160" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1160" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1161" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1161" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D1161" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1161" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F1161" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1161" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1161" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1162" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1162" s="3" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D1162" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1162" s="3" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F1162" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1162" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1162" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1163" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1163" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D1163" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1163" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1163" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1163" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1163" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1164" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1164" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D1164" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1164" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="F1164" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1164" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1164" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1165" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C1165" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D1165" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1165" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F1165" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1165" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1165" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1166" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E1166" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F1166" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G1166" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1166" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>